<commit_message>
corrected fastq xlsx fixture
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.12.fastq.xlsx
+++ b/tests/fixtures/orderforms/1508.12.fastq.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCC065D-C85D-9E4C-B73B-B5CBB5491983}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25580" yWindow="7860" windowWidth="25180" windowHeight="14060" tabRatio="262" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="25580" yWindow="7860" windowWidth="25180" windowHeight="14060" tabRatio="262" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="5" r:id="rId1"/>
@@ -13,7 +19,7 @@
     <sheet name="Genlista" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1688,20 +1694,20 @@
     <t>family1</t>
   </si>
   <si>
-    <t>prov 1</t>
-  </si>
-  <si>
-    <t>prov 2</t>
+    <t>prov1</t>
+  </si>
+  <si>
+    <t>prov2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="44" x14ac:knownFonts="1">
+  <fonts count="44">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2993,309 +2999,309 @@
     </xf>
   </cellXfs>
   <cellStyles count="304">
-    <cellStyle name="Excel Built-in Normal" xfId="45"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="287" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="291" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="293" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="295" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="297" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="299" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="301" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="303" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="134" builtinId="8"/>
-    <cellStyle name="Input" xfId="260" builtinId="20"/>
+    <cellStyle name="Excel Built-in Normal" xfId="45" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Följd hyperlänk" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="291" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="293" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="295" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="297" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="299" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="301" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="303" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="134" builtinId="8"/>
+    <cellStyle name="Indata" xfId="260" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3368,6 +3374,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3388,7 +3402,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3431,7 +3451,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3763,7 +3789,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3807,7 +3833,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3828,14 +3854,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="88" style="125" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" style="125" customWidth="1"/>
@@ -3853,7 +3879,7 @@
       <c r="D1" s="124"/>
       <c r="E1" s="58"/>
     </row>
-    <row r="2" spans="1:5" ht="16" hidden="1">
+    <row r="2" spans="1:5" ht="17" hidden="1">
       <c r="A2" s="124"/>
       <c r="B2" s="124"/>
       <c r="C2" s="124"/>
@@ -3890,12 +3916,12 @@
         <v>307</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19">
+    <row r="14" spans="1:5" ht="20">
       <c r="A14" s="72" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="16">
       <c r="A15" s="134" t="s">
         <v>324</v>
       </c>
@@ -3905,27 +3931,27 @@
         <v>365</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15">
+    <row r="18" spans="1:1" ht="16">
       <c r="A18" s="135" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="24">
+    <row r="19" spans="1:1" ht="28">
       <c r="A19" s="131" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="60">
+    <row r="20" spans="1:1" ht="70">
       <c r="A20" s="131" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="24">
+    <row r="21" spans="1:1" ht="28">
       <c r="A21" s="131" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15">
+    <row r="23" spans="1:1" ht="16">
       <c r="A23" s="135" t="s">
         <v>325</v>
       </c>
@@ -3935,54 +3961,54 @@
         <v>326</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="36">
+    <row r="25" spans="1:1" ht="42">
       <c r="A25" s="162" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="24">
+    <row r="26" spans="1:1" ht="28">
       <c r="A26" s="163" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="24">
+    <row r="27" spans="1:1" ht="28">
       <c r="A27" s="163" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="24">
+    <row r="28" spans="1:1" ht="28">
       <c r="A28" s="163" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="24">
+    <row r="29" spans="1:1" ht="28">
       <c r="A29" s="163" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="36">
+    <row r="30" spans="1:1" ht="56">
       <c r="A30" s="163" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="24">
+    <row r="31" spans="1:1" ht="28">
       <c r="A31" s="163" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="48">
+    <row r="32" spans="1:1" ht="56">
       <c r="A32" s="162" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="24">
+    <row r="33" spans="1:5" ht="28">
       <c r="A33" s="162" t="s">
         <v>344</v>
       </c>
       <c r="C33" s="131"/>
       <c r="E33" s="131"/>
     </row>
-    <row r="34" spans="1:5" ht="24">
+    <row r="34" spans="1:5" ht="42">
       <c r="A34" s="162" t="s">
         <v>334</v>
       </c>
@@ -4000,7 +4026,7 @@
       </c>
       <c r="E36" s="131"/>
     </row>
-    <row r="37" spans="1:5" ht="24">
+    <row r="37" spans="1:5" ht="28">
       <c r="A37" s="162" t="s">
         <v>345</v>
       </c>
@@ -4018,12 +4044,12 @@
         <v>364</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="36">
+    <row r="41" spans="1:5" ht="42">
       <c r="A41" s="162" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="24">
+    <row r="42" spans="1:5" ht="28">
       <c r="A42" s="162" t="s">
         <v>347</v>
       </c>
@@ -4036,12 +4062,12 @@
         <v>330</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="24">
+    <row r="45" spans="1:5" ht="28">
       <c r="A45" s="162" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="24">
+    <row r="46" spans="1:5" ht="28">
       <c r="A46" s="162" t="s">
         <v>349</v>
       </c>
@@ -4072,12 +4098,12 @@
         <v>366</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="24">
+    <row r="53" spans="1:1" ht="28">
       <c r="A53" s="162" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="24">
+    <row r="54" spans="1:1" ht="28">
       <c r="A54" s="162" t="s">
         <v>351</v>
       </c>
@@ -4165,7 +4191,7 @@
   </sheetData>
   <sheetProtection password="83BD" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="A14" r:id="rId1"/>
+    <hyperlink ref="A14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4179,17 +4205,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AL395"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="18" style="2" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
@@ -27386,7 +27412,7 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1"/>
+    <hyperlink ref="A7" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="1.05" bottom="1.05" header="0.79000000000000015" footer="0.79000000000000015"/>
   <pageSetup paperSize="9" scale="56" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -27397,79 +27423,79 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Genlista!$A$2:$A$35</xm:f>
           </x14:formula1>
           <xm:sqref>O15:O394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specify in the comments collumn if DSD sample!">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specify in the comments collumn if DSD sample!" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Sheet3!$G$1:$G$3</xm:f>
           </x14:formula1>
           <xm:sqref>P15:P394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>Sheet3!$K$1:$K$4</xm:f>
           </x14:formula1>
           <xm:sqref>J15:K394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>Sheet3!$D$1:$D$2</xm:f>
           </x14:formula1>
           <xm:sqref>H15:H394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>Sheet3!$N$1:$N$41</xm:f>
           </x14:formula1>
           <xm:sqref>G15:G394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>Sheet3!$E$1:$E$3</xm:f>
           </x14:formula1>
           <xm:sqref>E15:E394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>Sheet3!$A$1:$A$2</xm:f>
           </x14:formula1>
           <xm:sqref>B15:B394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>Sheet3!$O$1:$O$96</xm:f>
           </x14:formula1>
           <xm:sqref>M15:M394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="This is not a valid input (only yes/no is valid)">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="This is not a valid input (only yes/no is valid)" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>Sheet3!$D$1:$D$2</xm:f>
           </x14:formula1>
           <xm:sqref>V16:V394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="This is not a valid input (only yes/no is valid)">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="This is not a valid input (only yes/no is valid)" xr:uid="{00000000-0002-0000-0100-000009000000}">
           <x14:formula1>
             <xm:f>Sheet3!$D$1:$D$2</xm:f>
           </x14:formula1>
           <xm:sqref>V15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
           <x14:formula1>
             <xm:f>Sheet3!$C$1:$C$5</xm:f>
           </x14:formula1>
           <xm:sqref>C15:C394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
           <x14:formula1>
             <xm:f>Sheet3!$L$1:$L$8</xm:f>
           </x14:formula1>
           <xm:sqref>I15:I394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Make sure the information matches the valid Application tags in the information tab">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Make sure the information matches the valid Application tags in the information tab" xr:uid="{00000000-0002-0000-0100-00000C000000}">
           <x14:formula1>
             <xm:f>Sheet3!$B$1:$B$49</xm:f>
           </x14:formula1>
@@ -27485,14 +27511,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y103"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
@@ -27529,7 +27555,7 @@
       <c r="X1" s="148"/>
       <c r="Y1" s="148"/>
     </row>
-    <row r="2" spans="1:25" ht="22">
+    <row r="2" spans="1:25" ht="24">
       <c r="A2" s="149" t="s">
         <v>158</v>
       </c>
@@ -30904,12 +30930,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:A39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
@@ -31114,14 +31140,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AA96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="3" width="12.1640625" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Scout and Cancer together
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.12.fastq.xlsx
+++ b/tests/fixtures/orderforms/1508.12.fastq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCC065D-C85D-9E4C-B73B-B5CBB5491983}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6451551B-E88E-484E-A38F-3D6BCBA7EDFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25580" yWindow="7860" windowWidth="25180" windowHeight="14060" tabRatio="262" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24520" yWindow="7860" windowWidth="26240" windowHeight="14060" tabRatio="262" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4520" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4524" uniqueCount="415">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -1698,6 +1698,15 @@
   </si>
   <si>
     <t>prov2</t>
+  </si>
+  <si>
+    <t>plateA</t>
+  </si>
+  <si>
+    <t>extraction method</t>
+  </si>
+  <si>
+    <t>sample comment</t>
   </si>
 </sst>
 </file>
@@ -3789,7 +3798,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3833,7 +3842,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4211,8 +4220,8 @@
   </sheetPr>
   <dimension ref="A1:AL395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13"/>
@@ -4996,8 +5005,12 @@
         <v>170</v>
       </c>
       <c r="K15" s="95"/>
-      <c r="L15" s="138"/>
-      <c r="M15" s="94"/>
+      <c r="L15" s="138" t="s">
+        <v>412</v>
+      </c>
+      <c r="M15" s="94" t="s">
+        <v>51</v>
+      </c>
       <c r="N15" s="95"/>
       <c r="O15" s="94"/>
       <c r="P15" s="94"/>
@@ -5010,9 +5023,15 @@
         <v>162</v>
       </c>
       <c r="W15" s="97"/>
-      <c r="X15" s="94"/>
-      <c r="Y15" s="94"/>
-      <c r="Z15" s="94"/>
+      <c r="X15" s="94">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="94" t="s">
+        <v>413</v>
+      </c>
+      <c r="Z15" s="94" t="s">
+        <v>414</v>
+      </c>
       <c r="AA15" s="97"/>
       <c r="AB15" s="42" t="s">
         <v>25</v>

</xml_diff>